<commit_message>
updated MCS2 sheets with additional UC elements
</commit_message>
<xml_diff>
--- a/input/reg_health_wellbeing.xlsx
+++ b/input/reg_health_wellbeing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\andy_local\SimPaths project files\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2219F698-D79E-4541-A4E7-A159D929903F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D26B29-1931-46E6-A34C-3E7BD5442906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="2340" windowWidth="28770" windowHeight="13200" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UK_DHE_MCS1" sheetId="19" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="47">
   <si>
     <t>REGRESSOR</t>
   </si>
@@ -154,6 +154,21 @@
   </si>
   <si>
     <t>RealIncomeDecrease_D</t>
+  </si>
+  <si>
+    <t>D_Econ_benefits_UC_Lhw_ZERO</t>
+  </si>
+  <si>
+    <t>D_Econ_benefits_UC_Lhw_TEN</t>
+  </si>
+  <si>
+    <t>D_Econ_benefits_UC_Lhw_TWENTY</t>
+  </si>
+  <si>
+    <t>D_Econ_benefits_UC_Lhw_THIRTY</t>
+  </si>
+  <si>
+    <t>D_Econ_benefits_UC_Lhw_FORTY</t>
   </si>
 </sst>
 </file>
@@ -3354,16 +3369,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832F923C-A72E-4542-A215-4DEB3BB7E81E}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:O9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3394,8 +3411,23 @@
       <c r="J1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -3426,8 +3458,23 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -3458,8 +3505,23 @@
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3490,8 +3552,23 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -3522,8 +3599,23 @@
       <c r="J5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3554,8 +3646,23 @@
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -3586,8 +3693,23 @@
       <c r="J7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -3618,8 +3740,23 @@
       <c r="J8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -3649,6 +3786,256 @@
       </c>
       <c r="J9">
         <v>1.30250079019638E-2</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>-2.2400000000000002</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>9.0920710120782997E-2</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>-1.27</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0.40933881715951598</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>-1.0740000000000001</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0.23123340535193601</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>-0.55900000000000005</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0.22708142440649701</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14">
+        <v>-0.76900000000000002</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0.140625</v>
       </c>
     </row>
   </sheetData>
@@ -3659,16 +4046,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507D7AC2-8D5E-4487-A269-96C4EFD731AD}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3699,8 +4088,23 @@
       <c r="J1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -3731,8 +4135,23 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -3763,8 +4182,23 @@
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3795,8 +4229,23 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -3827,8 +4276,23 @@
       <c r="J5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3859,8 +4323,23 @@
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -3891,8 +4370,23 @@
       <c r="J7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -3923,8 +4417,23 @@
       <c r="J8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -3954,6 +4463,256 @@
       </c>
       <c r="J9">
         <v>1.3002974181362301E-2</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>-2.2400000000000002</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>9.0920710120782997E-2</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>-1.27</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0.40933881715951598</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>-1.0740000000000001</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0.23123340535193601</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>-0.55900000000000005</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0.22708142440649701</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14">
+        <v>-0.76900000000000002</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0.140625</v>
       </c>
     </row>
   </sheetData>
@@ -10615,7 +11374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3469CB-42ED-4984-ACB1-66223A508A16}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>